<commit_message>
added throttling to fix 429
</commit_message>
<xml_diff>
--- a/zipboard_help_articles.xlsx
+++ b/zipboard_help_articles.xlsx
@@ -13395,12 +13395,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Getting Started</t>
+          <t>User Management</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lack of a single, unified permissions matrix or concise table outlining the main differences in capabilities/permissions for all user roles (internal and external).</t>
+          <t>Lack of a single, unified permissions matrix for all user roles (Super Admin, Admin, Manager, Collaborator, Client, Guest Collaborator, Reviewer), including granular permissions for external roles and clarification of inconsistent naming ('Guest Collaborator' vs 'Guest Reviewer'). The 'Guest Collaborator' role is mentioned in an article title but not defined.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -13410,12 +13410,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Comprehensive User Role Permissions Matrix and Comparison</t>
+          <t>Understanding User Roles and Permissions in zipBoard: A Comprehensive Guide</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A unified permissions matrix is critical for administrators to quickly understand, compare, and correctly assign roles, preventing security risks and workflow inefficiencies due to incorrect access levels. This combines the need for a summary and a full matrix.</t>
+          <t>Users need a clear, single source to understand who can do what across all internal and external user types. Inconsistent naming, missing definitions, and a fragmented view of permissions cause significant confusion, impact security, and hinder effective user management and project setup.</t>
         </is>
       </c>
     </row>
@@ -13427,12 +13427,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Getting Started</t>
+          <t>Client Management</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Granular permissions for Client and Guest Reviewer roles are less defined compared to internal roles, leading to ambiguity about their specific capabilities.</t>
+          <t>The article on working with clients is severely lacking: it only references a video (which itself is missing), omits explicit text-based instructions for inviting clients, lacks screenshots for UI navigation, contains unclear terminology ('u' in permissions), and provides no information on accessing advanced sharing options or removing/revoking client access.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -13442,12 +13442,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Detailed Permissions for Client and Guest Reviewer Roles</t>
+          <t>Complete Guide to Client Collaboration and Management in zipBoard</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Lack of clear, granular permissions for external roles can create security vulnerabilities or prevent effective collaboration, as users are unsure of what actions these roles can perform.</t>
+          <t>This gap prevents users from effectively inviting, managing, and securing client access, which is a critical aspect of external collaboration. The reliance on a missing video and absence of text instructions create a major barrier to entry and ongoing client management.</t>
         </is>
       </c>
     </row>
@@ -13459,12 +13459,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Getting Started</t>
+          <t>Collaborator Management</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No definition or description of 'Guest Collaborator' as listed in the article title 'What’s the difference between Super Admin, Admin, Manager, Collaborator, Client, Guest Collaborator and Reviewer?'.</t>
+          <t>Help articles related to collaborators are ambiguous about their currency, lack detailed explanations of specific actions collaborators and reviewers can perform within a project, provide no information on managing existing collaborators (e.g., removing, changing roles, adding multiple), and omit troubleshooting steps for common invitation issues (e.g., email delivery, expired links).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -13474,12 +13474,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Defining the Guest Collaborator Role in zipBoard</t>
+          <t>Managing Collaborators and Reviewers: Invitation, Roles, and Troubleshooting</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>When a role is explicitly mentioned in the title of an article comparing roles, its absence from the content creates a significant gap in understanding and makes the article incomplete.</t>
+          <t>Effective collaboration is a core function of zipBoard. The current documentation leaves users uncertain about collaborator capabilities, unable to perform essential management tasks, and without recourse for common issues, leading to significant workflow interruptions.</t>
         </is>
       </c>
     </row>
@@ -13491,12 +13491,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>All About Clients</t>
+          <t>Core Features</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Missing instructions on how to access the 'access tab' for enhanced sharing with clients.</t>
+          <t>The article on reviewing web-hosted content lacks specifics on 'required details' when adding a URL, 'chosen permissions' for shareable links, an explanation of how collaborators provide feedback (e.g., annotation tools), and troubleshooting steps for inaccessible URLs or review issues. A referenced 'new updates' link is also missing.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -13506,12 +13506,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Accessing and Utilizing the Client 'Access Tab' for Enhanced Sharing</t>
+          <t>Guide to Reviewing Web Hosted Content with zipBoard: Setup, Feedback &amp; Troubleshooting</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>If a specific tab is crucial for an enhanced sharing feature, the lack of instructions on how to locate and use it directly blocks users from leveraging that functionality.</t>
+          <t>Reviewing web content is a fundamental feature of zipBoard. Missing details on setup, permission configuration, how to use feedback tools, and troubleshooting prevent users from effectively utilizing this core functionality and resolving common problems.</t>
         </is>
       </c>
     </row>
@@ -13523,12 +13523,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>All About Clients</t>
+          <t>Project Management</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>No information on how to remove clients or revoke shared access, which is critical for security and project management.</t>
+          <t>The article on project phase completion dates lacks detailed steps on how to set and edit dates (including saving changes), does not clarify the meaning of 'estimated' vs. 'actual' dates, provides no information on the implications or impact of these dates (e.g., reporting, notifications, workflow), and omits details on user permissions required to manage them.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -13538,12 +13538,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Removing Clients and Revoking Shared Access in zipBoard</t>
+          <t>Managing Project Phase Completion Dates in zipBoard: Setting, Impact, and Permissions</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The ability to manage the lifecycle of client access, including removal and revocation, is fundamental for maintaining data security and adapting to changing project requirements.</t>
+          <t>Completion dates are central to project tracking and workflow management. The absence of 'how-to' steps, 'why-it-matters' context, and permission details makes it difficult for users to accurately set, understand, and leverage this feature for effective project oversight.</t>
         </is>
       </c>
     </row>

</xml_diff>